<commit_message>
Able to create an Excel file as a stream from a List<List<Object>>
</commit_message>
<xml_diff>
--- a/convertExcel/bin/Debug/Empty.xlsx
+++ b/convertExcel/bin/Debug/Empty.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <x:workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ama\Documents\LINQPad Queries\convertExcel\convertExcel\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:calcPr calcId="152511"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>